<commit_message>
Added new table and doc downloading
</commit_message>
<xml_diff>
--- a/bulletin/macroeconomics/static/macroeconomics/tables/labor_market_statistics.xlsx
+++ b/bulletin/macroeconomics/static/macroeconomics/tables/labor_market_statistics.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,468 +439,459 @@
       <c r="E1" t="n">
         <v>2022</v>
       </c>
-      <c r="F1" t="n">
-        <v>2023</v>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>2023
+1 кв</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1 кв</t>
-        </is>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Рабочая сила</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9221.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9180.799999999999</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9256.799999999999</v>
+      </c>
+      <c r="E2" t="n">
+        <v>9429.799999999999</v>
+      </c>
+      <c r="F2" t="n">
+        <v>9485.299999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Рабочая сила</t>
+          <t>Занятость (тыс. человек)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9221.5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>9180.799999999999</v>
-      </c>
-      <c r="D3" t="n">
-        <v>9256.799999999999</v>
-      </c>
-      <c r="E3" t="n">
-        <v>9429.799999999999</v>
-      </c>
+        <v>8780.799999999999</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>9485.299999999999</v>
+        <v>9031.9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Занятость (тыс. человек)</t>
+          <t>Сельское, лесное и рыбное хозяйство</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8780.799999999999</v>
+        <v>1184.7</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>9031.9</v>
+        <v>1036.4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Сельское, лесное и рыбное хозяйство</t>
+          <t>Горнодобывающая промышленность</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1184.7</v>
+        <v>279.9</v>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>1036.4</v>
+        <v>276.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Горнодобывающая промышленность</t>
+          <t>Обрабатывающая промышленность</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>279.9</v>
+        <v>583.6</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>276.7</v>
+        <v>615.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Обрабатывающая промышленность</t>
+          <t>Снабжение электроэнергией</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>583.6</v>
+        <v>150.2</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>615.6</v>
+        <v>158.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Снабжение электроэнергией</t>
+          <t>Водоснабжение</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>150.2</v>
+        <v>81.2</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>158.5</v>
+        <v>87.90000000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Водоснабжение</t>
+          <t>Строительство</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>81.2</v>
+        <v>635.6</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>87.90000000000001</v>
+        <v>623.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Строительство</t>
+          <t>Оптовая и розничная торговля</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>635.6</v>
+        <v>1431.1</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>623.5</v>
+        <v>1559.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Оптовая и розничная торговля</t>
+          <t>Транспорт и складирование</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1431.1</v>
+        <v>637.9</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>1559.8</v>
+        <v>645.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Транспорт и складирование</t>
+          <t>Предоставление услуг по проживанию и питанию</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>637.9</v>
+        <v>196.9</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>645.1</v>
+        <v>211.9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Предоставление услуг по проживанию и питанию</t>
+          <t>Информация и связь</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>196.9</v>
+        <v>161.7</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>211.9</v>
+        <v>182.1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Информация и связь</t>
+          <t>Финансовая и страховая деятельность</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>161.7</v>
+        <v>190.5</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>182.1</v>
+        <v>199.7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Финансовая и страховая деятельность</t>
+          <t>Операции с недвижимым имуществом</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>190.5</v>
+        <v>154.5</v>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>199.7</v>
+        <v>150.4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Операции с недвижимым имуществом</t>
+          <t>Профессиональная, научная и техническая деятельность</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>154.5</v>
+        <v>256.4</v>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>150.4</v>
+        <v>283.7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Профессиональная, научная и техническая деятельность</t>
+          <t>Деятельность в области административного и вспомогательного обслуживания</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>256.4</v>
+        <v>292.3</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>283.7</v>
+        <v>267.3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Деятельность в области административного и вспомогательного обслуживания</t>
+          <t>Государственное управление и оборона</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>292.3</v>
+        <v>495.3</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>267.3</v>
+        <v>508.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Государственное управление и оборона</t>
+          <t>Образование</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>495.3</v>
+        <v>1108.7</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>508.7</v>
+        <v>1166.4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Образование</t>
+          <t>Здравоохранение и социальное обслуживание населения</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1108.7</v>
+        <v>502.7</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>1166.4</v>
+        <v>562.4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Здравоохранение и социальное обслуживание населения</t>
+          <t>Искусство, развлечения и отдых</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>502.7</v>
+        <v>142</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>562.4</v>
+        <v>133.2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Искусство, развлечения и отдых</t>
+          <t>Предоставление прочих видов услуг</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>142</v>
+        <v>295.8</v>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>133.2</v>
+        <v>362.8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Предоставление прочих видов услуг</t>
+          <t>Наемные работники, тыс. человек</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>295.8</v>
+        <v>6697.6</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>362.8</v>
-      </c>
+      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Наемные работники, тыс. человек</t>
+          <t>Самозанятые, тыс. человек</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>6697.6</v>
+        <v>2099.2</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>2131.5</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Самозанятые, тыс. человек</t>
+          <t>Численность безработных, тыс. человек</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2099.2</v>
-      </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+        <v>440.7</v>
+      </c>
+      <c r="C25" t="n">
+        <v>448.8</v>
+      </c>
+      <c r="D25" t="n">
+        <v>449.6</v>
+      </c>
+      <c r="E25" t="n">
+        <v>458.3</v>
+      </c>
       <c r="F25" t="n">
-        <v>2131.5</v>
+        <v>453.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Численность безработных, тыс. человек</t>
+          <t>Уровень безработицы, %</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>440.7</v>
+        <v>4.8</v>
       </c>
       <c r="C26" t="n">
-        <v>448.8</v>
+        <v>4.9</v>
       </c>
       <c r="D26" t="n">
-        <v>449.6</v>
+        <v>4.9</v>
       </c>
       <c r="E26" t="n">
-        <v>458.3</v>
-      </c>
-      <c r="F26" t="n">
-        <v>453.5</v>
-      </c>
+        <v>4.9</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Уровень безработицы, %</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="C27" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="D27" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="E27" t="n">
-        <v>4.9</v>
-      </c>
+          <t>Доходы населения (на душу населения в год, тенге)</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Доходы населения (на душу населения в год, тенге)</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
           <t>Средняя заработная плата в тенге</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B28" t="n">
         <v>186.8</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C28" t="n">
         <v>213</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D28" t="n">
         <v>250.3</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E28" t="n">
         <v>309.9</v>
       </c>
-      <c r="F29" t="n">
-        <v>345.4</v>
+      <c r="F28" t="n">
+        <v>345.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>